<commit_message>
added new noise data
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_noise_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_noise_Runsheet_Bing.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC/bing_data/speed_acc_child_noise/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="300" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="114">
   <si>
     <t>subid</t>
   </si>
@@ -45,6 +50,132 @@
     <t>comments</t>
   </si>
   <si>
+    <t>SPEED_ACC_NOISE_1</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_2</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_3</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_4</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_5</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_6</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_7</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_8</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_9</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_10</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_11</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_12</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_13</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_14</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_15</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_16</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_17</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_18</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_19</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_20</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_21</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_22</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_23</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_24</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_25</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_26</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_27</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_28</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_29</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_30</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_31</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_32</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_33</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_34</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_35</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_36</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_37</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_38</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_39</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_40</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_41</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_42</t>
+  </si>
+  <si>
     <t>order4</t>
   </si>
   <si>
@@ -111,136 +242,130 @@
     <t>stopped playing at the end</t>
   </si>
   <si>
-    <t>SPEED_ACC_CHILD_NOISE_1</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_2</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_3</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_4</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_5</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_6</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_7</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_8</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_9</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_10</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_11</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_12</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_13</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_14</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_15</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_16</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_17</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_18</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_19</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_20</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_21</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_22</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_23</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_24</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_25</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_26</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_27</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_28</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_29</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_30</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_31</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_32</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_33</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_34</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_35</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_36</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_37</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_38</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_39</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_40</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_41</t>
-  </si>
-  <si>
-    <t>SPEED_ACC_CHILD_NOISE_42</t>
-  </si>
-  <si>
-    <t>exclude</t>
-  </si>
-  <si>
-    <t>keep</t>
+    <t xml:space="preserve">stopped early, also didn't calibrate…and I didn't take her name tag off </t>
+  </si>
+  <si>
+    <t>got frustrated towards the end</t>
+  </si>
+  <si>
+    <t>she kept saying "on the right/left side!" and "yes"</t>
+  </si>
+  <si>
+    <t>stopped early, she said the noise hurt her ears</t>
+  </si>
+  <si>
+    <t>stopped early</t>
+  </si>
+  <si>
+    <t>went well! got a little bored towards the end</t>
+  </si>
+  <si>
+    <t>went well! got distracted towards the end</t>
+  </si>
+  <si>
+    <t>distracted during calibration, only one eye calibrated.</t>
+  </si>
+  <si>
+    <t>seemed a little stunned by the noise, distracted by the cord for the headphones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">went well! mom said that she makes hand movements like she's trying to grab something when she sees something she likes </t>
+  </si>
+  <si>
+    <t>did not go well, she started crying a few trials in</t>
+  </si>
+  <si>
+    <t>touched the screen like an ipad, may have interfered with eye tracking, also super close to the screen</t>
+  </si>
+  <si>
+    <t>slouched in the chair, but went well!</t>
+  </si>
+  <si>
+    <t>stopped early, but made it through most of the trials</t>
+  </si>
+  <si>
+    <t>very distracted, humming a lot</t>
+  </si>
+  <si>
+    <t>calibration slightly off, got bored towards the end</t>
+  </si>
+  <si>
+    <t>very distracted, messing with the headphone, they fell off for a little while, said "it's too noisy!"</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_43</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_44</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_45</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_46</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_47</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_48</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_49</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_50</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_51</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_52</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_53</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_54</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_55</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_56</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_57</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_58</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_59</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_60</t>
+  </si>
+  <si>
+    <t>touching screen like an ipad, but went well!</t>
+  </si>
+  <si>
+    <t>did not want to wear headphones, couldn't hear the noise trials and stopped early</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_61</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_62</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_63</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_64</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_NOISE_65</t>
   </si>
 </sst>
 </file>
@@ -290,13 +415,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -372,7 +495,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -405,7 +528,6 @@
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -438,7 +560,6 @@
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -774,19 +895,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -811,13 +932,10 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>42934</v>
@@ -826,21 +944,18 @@
         <v>41164</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>42934</v>
@@ -849,21 +964,18 @@
         <v>41124</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>42934</v>
@@ -872,21 +984,18 @@
         <v>41014</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>42934</v>
@@ -895,21 +1004,18 @@
         <v>41605</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>42936</v>
@@ -918,21 +1024,18 @@
         <v>40974</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>42936</v>
@@ -941,21 +1044,18 @@
         <v>41267</v>
       </c>
       <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>14</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A8" t="s">
-        <v>36</v>
       </c>
       <c r="B8" s="2">
         <v>42936</v>
@@ -964,21 +1064,18 @@
         <v>41194</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>42936</v>
@@ -987,21 +1084,18 @@
         <v>41569</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>42936</v>
@@ -1010,21 +1104,18 @@
         <v>41192</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>42936</v>
@@ -1033,21 +1124,18 @@
         <v>41522</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
         <v>42941</v>
@@ -1056,21 +1144,18 @@
         <v>41246</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="H12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
         <v>19</v>
-      </c>
-      <c r="I12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A13" t="s">
-        <v>41</v>
       </c>
       <c r="B13" s="1">
         <v>42941</v>
@@ -1079,21 +1164,18 @@
         <v>41683</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>42941</v>
@@ -1102,21 +1184,18 @@
         <v>41659</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>42941</v>
@@ -1125,21 +1204,18 @@
         <v>41072</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>42941</v>
@@ -1148,21 +1224,18 @@
         <v>41616</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1">
         <v>42941</v>
@@ -1171,21 +1244,18 @@
         <v>41055</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
         <v>42941</v>
@@ -1194,21 +1264,18 @@
         <v>41568</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>25</v>
-      </c>
-      <c r="I18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A19" t="s">
-        <v>47</v>
       </c>
       <c r="B19" s="1">
         <v>42943</v>
@@ -1217,21 +1284,18 @@
         <v>41340</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="H19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
         <v>26</v>
-      </c>
-      <c r="I19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A20" t="s">
-        <v>48</v>
       </c>
       <c r="B20" s="1">
         <v>42943</v>
@@ -1240,21 +1304,18 @@
         <v>41814</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="H20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>27</v>
-      </c>
-      <c r="I20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A21" t="s">
-        <v>49</v>
       </c>
       <c r="B21" s="1">
         <v>42943</v>
@@ -1263,21 +1324,18 @@
         <v>40855</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>28</v>
-      </c>
-      <c r="I21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>50</v>
       </c>
       <c r="B22" s="1">
         <v>42943</v>
@@ -1286,305 +1344,703 @@
         <v>41242</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="H22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="I22" t="s">
+      <c r="B23" s="1">
+        <v>42948</v>
+      </c>
+      <c r="C23" s="1">
+        <v>41082</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42948</v>
+      </c>
+      <c r="C24" s="1">
+        <v>41584</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42948</v>
+      </c>
+      <c r="C25" s="1">
+        <v>41660</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A23" t="s">
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42950</v>
+      </c>
+      <c r="C26" s="1">
+        <v>41639</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="G23" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A24" t="s">
+      <c r="H26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42950</v>
+      </c>
+      <c r="C27" s="1">
+        <v>41779</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="G24" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A25" t="s">
+      <c r="H27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42950</v>
+      </c>
+      <c r="C28" s="1">
+        <v>41594</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42961</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42961</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="G25" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="G26" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="G27" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A28" t="s">
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42961</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="G28" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="G29" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="G30" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="E31">
+        <v>4</v>
+      </c>
       <c r="G31" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" customHeight="1">
+        <v>50</v>
+      </c>
+      <c r="H31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42962</v>
+      </c>
       <c r="C32" s="1"/>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
       <c r="G32" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="12.75" customHeight="1">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42962</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42962</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="1">
+        <v>42962</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="1">
+        <v>42963</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="2">
+        <v>42963</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H37" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="G33" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="G34" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="G35" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="G36" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="G37" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="12.75" customHeight="1">
+    </row>
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="B38" s="2">
+        <v>42963</v>
+      </c>
       <c r="C38" s="2"/>
+      <c r="D38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
       <c r="G38" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="12.75" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="H38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="B39" s="2">
+        <v>42963</v>
+      </c>
       <c r="C39" s="2"/>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
       <c r="G39" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="12.75" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="H39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B40" s="2">
+        <v>42963</v>
+      </c>
       <c r="C40" s="2"/>
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
       <c r="G40" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="12.75" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="H40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="B41" s="2">
+        <v>42963</v>
+      </c>
       <c r="C41" s="2"/>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
       <c r="G41" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="12.75" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="H41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="B42" s="2">
+        <v>42963</v>
+      </c>
       <c r="C42" s="2"/>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
       <c r="G42" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="12.75" customHeight="1">
+        <v>50</v>
+      </c>
+      <c r="H42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="B43" s="2">
+        <v>42964</v>
+      </c>
       <c r="C43" s="2"/>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
       <c r="G43" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B44" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="H43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="2">
+        <v>42964</v>
+      </c>
       <c r="C44" s="2"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B45" s="2"/>
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="2">
+        <v>42964</v>
+      </c>
       <c r="C45" s="2"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B46" s="2"/>
+      <c r="D45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="2">
+        <v>42964</v>
+      </c>
       <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" ht="12.75" customHeight="1">
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" ht="12.75" customHeight="1">
+      <c r="G47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>94</v>
+      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>95</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>100</v>
+      </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>101</v>
+      </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>104</v>
+      </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-    </row>
-    <row r="60" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
+      <c r="G60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+      <c r="G61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="G62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="G63" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>111</v>
+      </c>
+      <c r="G64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>112</v>
+      </c>
+      <c r="G65" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="G66" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added models with child's age as continous predictor
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_noise_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_noise_Runsheet_Bing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24380" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25100" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -376,8 +376,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="76">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -454,8 +463,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -466,8 +481,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="76">
+  <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -505,6 +523,9 @@
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -542,6 +563,9 @@
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -879,13 +903,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B51"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -959,7 +987,7 @@
         <v>56</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F28" si="0">DATEDIF(C3,B3,"y")</f>
+        <f t="shared" ref="F3:F51" si="0">DATEDIF(C3,B3,"y")</f>
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1654,11 +1682,14 @@
       <c r="B29" s="1">
         <v>42961</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1">
+        <v>41543</v>
+      </c>
       <c r="D29" t="s">
         <v>56</v>
       </c>
       <c r="F29">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -1678,12 +1709,15 @@
       <c r="B30" s="1">
         <v>42961</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1">
+        <v>41505</v>
+      </c>
       <c r="D30" t="s">
         <v>56</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>53</v>
@@ -1702,11 +1736,14 @@
       <c r="B31" s="1">
         <v>42961</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1">
+        <v>41194</v>
+      </c>
       <c r="D31" t="s">
         <v>56</v>
       </c>
       <c r="F31">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -1726,11 +1763,14 @@
       <c r="B32" s="1">
         <v>42962</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" s="1">
+        <v>41673</v>
+      </c>
       <c r="D32" t="s">
         <v>54</v>
       </c>
       <c r="F32">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -1750,11 +1790,14 @@
       <c r="B33" s="1">
         <v>42962</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" s="1">
+        <v>41739</v>
+      </c>
       <c r="D33" t="s">
         <v>54</v>
       </c>
       <c r="F33">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -1774,11 +1817,14 @@
       <c r="B34" s="1">
         <v>42962</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1">
+        <v>41092</v>
+      </c>
       <c r="D34" t="s">
         <v>54</v>
       </c>
       <c r="F34">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -1798,11 +1844,14 @@
       <c r="B35" s="1">
         <v>42962</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1">
+        <v>41673</v>
+      </c>
       <c r="D35" t="s">
         <v>54</v>
       </c>
       <c r="F35">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -1822,11 +1871,14 @@
       <c r="B36" s="1">
         <v>42963</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1">
+        <v>41130</v>
+      </c>
       <c r="D36" t="s">
         <v>54</v>
       </c>
       <c r="F36">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -1846,11 +1898,14 @@
       <c r="B37" s="2">
         <v>42963</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2">
+        <v>41803</v>
+      </c>
       <c r="D37" t="s">
         <v>54</v>
       </c>
       <c r="F37">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G37" s="3" t="s">
@@ -1870,11 +1925,14 @@
       <c r="B38" s="2">
         <v>42963</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2">
+        <v>41081</v>
+      </c>
       <c r="D38" t="s">
         <v>54</v>
       </c>
       <c r="F38">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -1894,11 +1952,14 @@
       <c r="B39" s="2">
         <v>42963</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2">
+        <v>41638</v>
+      </c>
       <c r="D39" t="s">
         <v>56</v>
       </c>
       <c r="F39">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G39" s="3" t="s">
@@ -1918,11 +1979,14 @@
       <c r="B40" s="2">
         <v>42963</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="2">
+        <v>41374</v>
+      </c>
       <c r="D40" t="s">
         <v>56</v>
       </c>
       <c r="F40">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -1942,11 +2006,14 @@
       <c r="B41" s="2">
         <v>42963</v>
       </c>
-      <c r="C41" s="2"/>
+      <c r="C41" s="2">
+        <v>41510</v>
+      </c>
       <c r="D41" t="s">
         <v>56</v>
       </c>
       <c r="F41">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G41" s="3" t="s">
@@ -1966,11 +2033,14 @@
       <c r="B42" s="2">
         <v>42963</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2">
+        <v>41121</v>
+      </c>
       <c r="D42" t="s">
         <v>54</v>
       </c>
       <c r="F42">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -1990,11 +2060,14 @@
       <c r="B43" s="2">
         <v>42964</v>
       </c>
-      <c r="C43" s="2"/>
+      <c r="C43" s="2">
+        <v>41813</v>
+      </c>
       <c r="D43" t="s">
         <v>56</v>
       </c>
       <c r="F43">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -2014,11 +2087,14 @@
       <c r="B44" s="2">
         <v>42964</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2">
+        <v>41551</v>
+      </c>
       <c r="D44" t="s">
         <v>56</v>
       </c>
       <c r="F44">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -2038,11 +2114,14 @@
       <c r="B45" s="2">
         <v>42964</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="4">
+        <v>41551</v>
+      </c>
       <c r="D45" t="s">
         <v>56</v>
       </c>
       <c r="F45">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -2062,11 +2141,14 @@
       <c r="B46" s="2">
         <v>42964</v>
       </c>
-      <c r="C46" s="2"/>
+      <c r="C46" s="2">
+        <v>41007</v>
+      </c>
       <c r="D46" t="s">
         <v>56</v>
       </c>
       <c r="F46">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G46" t="s">
@@ -2086,11 +2168,14 @@
       <c r="B47" s="2">
         <v>42964</v>
       </c>
-      <c r="C47" s="2"/>
+      <c r="C47" s="2">
+        <v>41128</v>
+      </c>
       <c r="D47" t="s">
         <v>54</v>
       </c>
       <c r="F47">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G47" t="s">
@@ -2110,11 +2195,14 @@
       <c r="B48" s="2">
         <v>42964</v>
       </c>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2">
+        <v>41208</v>
+      </c>
       <c r="D48" t="s">
         <v>56</v>
       </c>
       <c r="F48">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G48" t="s">
@@ -2134,11 +2222,14 @@
       <c r="B49" s="2">
         <v>42964</v>
       </c>
-      <c r="C49" s="2"/>
+      <c r="C49" s="2">
+        <v>41018</v>
+      </c>
       <c r="D49" t="s">
         <v>56</v>
       </c>
       <c r="F49">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G49" t="s">
@@ -2158,11 +2249,14 @@
       <c r="B50" s="2">
         <v>42965</v>
       </c>
-      <c r="C50" s="2"/>
+      <c r="C50" s="2">
+        <v>41339</v>
+      </c>
       <c r="D50" t="s">
         <v>56</v>
       </c>
       <c r="F50">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G50" t="s">
@@ -2182,11 +2276,14 @@
       <c r="B51" s="2">
         <v>42965</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2">
+        <v>41272</v>
+      </c>
       <c r="D51" t="s">
         <v>54</v>
       </c>
       <c r="F51">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G51" t="s">

</xml_diff>